<commit_message>
Adding Second Shooter Motor
</commit_message>
<xml_diff>
--- a/2579 - Got'em/src/org/frc/team2579/subsystems/JoyNonlinearityCalc.xlsx
+++ b/2579 - Got'em/src/org/frc/team2579/subsystems/JoyNonlinearityCalc.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\2017-Got-em\2579 - Got'em\src\org\frc\team2579\subsystems\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Input</t>
   </si>
@@ -40,15 +38,34 @@
   <si>
     <t>Desire</t>
   </si>
+  <si>
+    <t>C3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,13 +88,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -94,7 +115,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -142,26 +163,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -239,8 +240,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.18378280839895014"/>
-                  <c:y val="-0.18666411490230389"/>
+                  <c:x val="0.18378280839895"/>
+                  <c:y val="-0.186664114902304"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -280,37 +281,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -322,43 +323,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>66</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4E87-45CC-BF61-E32C7ED7EC97}"/>
             </c:ext>
@@ -372,11 +373,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="478011551"/>
-        <c:axId val="478012383"/>
+        <c:axId val="2119716504"/>
+        <c:axId val="2119720232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="478011551"/>
+        <c:axId val="2119716504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,12 +434,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="478012383"/>
+        <c:crossAx val="2119720232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="478012383"/>
+        <c:axId val="2119720232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +496,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="478011551"/>
+        <c:crossAx val="2119716504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -542,562 +543,6 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,7 +623,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1213,7 +658,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1390,7 +835,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1401,12 +846,12 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1417,25 +862,25 @@
         <v>2</v>
       </c>
       <c r="E1">
-        <v>0.75</v>
+        <v>1.1599999999999999E-2</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <f>$E$1*EXP($E$2*A2)</f>
-        <v>0.75</v>
+        <f>$E$1*A2^2+$E$2*A2+$E$3</f>
+        <v>4.3705999999999996</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2">
-        <v>0.05</v>
+        <v>-0.28499999999999998</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -1444,13 +889,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B12" si="0">$E$1*EXP($E$2*A3)</f>
-        <v>1.2365409530250961</v>
+        <f t="shared" ref="B3:B12" si="0">$E$1*A3^2+$E$2*A3+$E$3</f>
+        <v>2.6806000000000001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>4.3705999999999996</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1459,142 +910,142 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>20</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>2.0387113713442839</v>
+        <v>3.3106</v>
       </c>
       <c r="H4">
         <v>10</v>
       </c>
       <c r="I4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>30</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>3.3612668027535486</v>
+        <v>6.2606000000000002</v>
       </c>
       <c r="H5">
         <v>20</v>
       </c>
       <c r="I5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>40</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>5.5417920741979874</v>
+        <v>11.5306</v>
       </c>
       <c r="H6">
         <v>30</v>
       </c>
       <c r="I6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>50</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>9.1368704705276045</v>
+        <v>19.120599999999996</v>
       </c>
       <c r="H7">
         <v>40</v>
       </c>
       <c r="I7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>60</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>15.064152692390751</v>
+        <v>29.0306</v>
       </c>
       <c r="H8">
         <v>50</v>
       </c>
       <c r="I8">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>70</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>24.836588969019232</v>
+        <v>41.260599999999997</v>
       </c>
       <c r="H9">
         <v>60</v>
       </c>
       <c r="I9">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>80</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>40.948612524858177</v>
+        <v>55.810599999999994</v>
       </c>
       <c r="H10">
         <v>70</v>
       </c>
       <c r="I10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>90</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>67.512848475391365</v>
+        <v>72.680599999999998</v>
       </c>
       <c r="H11">
         <v>80</v>
       </c>
       <c r="I11">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>100</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>111.30986932693244</v>
+        <v>91.870599999999982</v>
       </c>
       <c r="H12">
         <v>90</v>
       </c>
       <c r="I12">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="H13">
         <v>100</v>
       </c>
@@ -1604,6 +1055,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>